<commit_message>
Eta.fu --> eta.fu, Phi.u --> phi.u
</commit_message>
<xml_diff>
--- a/inst/extdata/Machine Examples/Machine_Example/Machine_Example.xlsx
+++ b/inst/extdata/Machine Examples/Machine_Example/Machine_Example.xlsx
@@ -1,27 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B22C274-17AC-764D-B44C-D725A2DF6730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="3" r:id="rId1"/>
     <sheet name="FIN_ETA" sheetId="2" r:id="rId2"/>
     <sheet name="UNEP_2017" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="33">
   <si>
     <t>Country</t>
   </si>
@@ -71,9 +81,6 @@
     <t>Eta.fu</t>
   </si>
   <si>
-    <t>Phi.u</t>
-  </si>
-  <si>
     <t>UNEP (2017) - Energy-Efficient Electric Motors and Motor Systems</t>
   </si>
   <si>
@@ -117,12 +124,18 @@
   </si>
   <si>
     <t>PCM</t>
+  </si>
+  <si>
+    <t>eta.fu</t>
+  </si>
+  <si>
+    <t>phi.u</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -275,7 +288,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2 3" xfId="1"/>
+    <cellStyle name="Normal 2 2 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -307,7 +320,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -345,7 +364,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -633,21 +658,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" customWidth="1"/>
-    <col min="3" max="3" width="54.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" customWidth="1"/>
+    <col min="3" max="3" width="54.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -658,7 +683,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -669,7 +694,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -684,26 +709,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BI11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="6"/>
-    <col min="2" max="2" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="9.1640625" style="6"/>
+    <col min="2" max="2" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="26.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="6" customWidth="1"/>
+    <col min="7" max="7" width="11.5" style="6" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:61" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
@@ -711,18 +736,18 @@
       <c r="C1" s="9"/>
       <c r="F1" s="9"/>
     </row>
-    <row r="2" spans="1:61" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:61" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>28</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>1</v>
@@ -731,7 +756,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H2" s="11">
         <v>1960</v>
@@ -896,18 +921,18 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="D3" s="14" t="s">
         <v>30</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>31</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>12</v>
@@ -916,7 +941,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="H3" s="12">
         <f t="array" ref="H3:BI3">TRANSPOSE(UNEP_2017!G5:G58)</f>
@@ -1082,18 +1107,18 @@
         <v>0.95799999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="D4" s="14" t="s">
         <v>30</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>31</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>12</v>
@@ -1102,7 +1127,7 @@
         <v>13</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="H4" s="6">
         <v>1</v>
@@ -1267,37 +1292,37 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.2">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.2">
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.2">
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
     </row>
-    <row r="8" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.2">
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
     </row>
-    <row r="9" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.2">
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
     </row>
-    <row r="10" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.2">
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
     </row>
-    <row r="11" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.2">
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -1308,38 +1333,38 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>1</v>
@@ -1348,7 +1373,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>1</v>
@@ -1357,15 +1382,15 @@
         <v>15</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>1960</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="6">
         <v>0.88</v>
@@ -1374,22 +1399,22 @@
         <v>1960</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G5" s="6">
         <f>C5</f>
         <v>0.88</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>1980</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="6">
         <v>0.9</v>
@@ -1398,22 +1423,22 @@
         <v>1961</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6" s="7">
         <f>G5+(($G$25-$G$5)/($E$25-$E$5))</f>
         <v>0.88100000000000001</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>1990</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="6">
         <v>0.90200000000000002</v>
@@ -1422,22 +1447,22 @@
         <v>1962</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G7" s="7">
         <f t="shared" ref="G7:G24" si="0">G6+(($G$25-$G$5)/($E$25-$E$5))</f>
         <v>0.88200000000000001</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>2000</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="6">
         <v>0.93899999999999995</v>
@@ -1446,22 +1471,22 @@
         <v>1963</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G8" s="7">
         <f t="shared" si="0"/>
         <v>0.88300000000000001</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>2010</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="6">
         <v>0.95099999999999996</v>
@@ -1470,22 +1495,22 @@
         <v>1964</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G9" s="7">
         <f t="shared" si="0"/>
         <v>0.88400000000000001</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>2013</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="6">
         <v>0.95799999999999996</v>
@@ -1494,739 +1519,739 @@
         <v>1965</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G10" s="7">
         <f t="shared" si="0"/>
         <v>0.88500000000000001</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E11" s="6">
         <v>1966</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G11" s="7">
         <f t="shared" si="0"/>
         <v>0.88600000000000001</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E12" s="6">
         <v>1967</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G12" s="7">
         <f t="shared" si="0"/>
         <v>0.88700000000000001</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E13" s="6">
         <v>1968</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G13" s="7">
         <f t="shared" si="0"/>
         <v>0.88800000000000001</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E14" s="6">
         <v>1969</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G14" s="7">
         <f t="shared" si="0"/>
         <v>0.88900000000000001</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E15" s="6">
         <v>1970</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G15" s="7">
         <f t="shared" si="0"/>
         <v>0.89</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E16" s="6">
         <v>1971</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G16" s="7">
         <f t="shared" si="0"/>
         <v>0.89100000000000001</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E17" s="6">
         <v>1972</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G17" s="7">
         <f t="shared" si="0"/>
         <v>0.89200000000000002</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E18" s="6">
         <v>1973</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G18" s="7">
         <f t="shared" si="0"/>
         <v>0.89300000000000002</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E19" s="6">
         <v>1974</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G19" s="7">
         <f t="shared" si="0"/>
         <v>0.89400000000000002</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E20" s="6">
         <v>1975</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G20" s="7">
         <f t="shared" si="0"/>
         <v>0.89500000000000002</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E21" s="6">
         <v>1976</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G21" s="7">
         <f t="shared" si="0"/>
         <v>0.89600000000000002</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E22" s="6">
         <v>1977</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G22" s="7">
         <f t="shared" si="0"/>
         <v>0.89700000000000002</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E23" s="6">
         <v>1978</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G23" s="7">
         <f t="shared" si="0"/>
         <v>0.89800000000000002</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E24" s="6">
         <v>1979</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G24" s="7">
         <f t="shared" si="0"/>
         <v>0.89900000000000002</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E25" s="6">
         <v>1980</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G25" s="6">
         <f>C6</f>
         <v>0.9</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="5:8" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E26" s="6">
         <v>1981</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G26" s="7">
         <f>G25+(($G$35-$G$25)/($E$35-$E$25))</f>
         <v>0.9002</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E27" s="6">
         <v>1982</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G27" s="7">
         <f t="shared" ref="G27:G34" si="1">G26+(($G$35-$G$25)/($E$35-$E$25))</f>
         <v>0.90039999999999998</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E28" s="6">
         <v>1983</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G28" s="7">
         <f t="shared" si="1"/>
         <v>0.90059999999999996</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E29" s="6">
         <v>1984</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G29" s="7">
         <f t="shared" si="1"/>
         <v>0.90079999999999993</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E30" s="6">
         <v>1985</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G30" s="7">
         <f t="shared" si="1"/>
         <v>0.90099999999999991</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E31" s="6">
         <v>1986</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G31" s="7">
         <f t="shared" si="1"/>
         <v>0.90119999999999989</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E32" s="6">
         <v>1987</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G32" s="7">
         <f t="shared" si="1"/>
         <v>0.90139999999999987</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E33" s="6">
         <v>1988</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G33" s="7">
         <f t="shared" si="1"/>
         <v>0.90159999999999985</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E34" s="6">
         <v>1989</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G34" s="7">
         <f t="shared" si="1"/>
         <v>0.90179999999999982</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E35" s="6">
         <v>1990</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G35" s="6">
         <f>C7</f>
         <v>0.90200000000000002</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="5:8" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E36" s="6">
         <v>1991</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G36" s="7">
         <f>G35+(($G$45-$G$35)/($E$45-$E$35))</f>
         <v>0.90570000000000006</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E37" s="6">
         <v>1992</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G37" s="7">
         <f t="shared" ref="G37:G44" si="2">G36+(($G$45-$G$35)/($E$45-$E$35))</f>
         <v>0.9094000000000001</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E38" s="6">
         <v>1993</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G38" s="7">
         <f t="shared" si="2"/>
         <v>0.91310000000000013</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E39" s="6">
         <v>1994</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G39" s="7">
         <f t="shared" si="2"/>
         <v>0.91680000000000017</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E40" s="6">
         <v>1995</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G40" s="7">
         <f t="shared" si="2"/>
         <v>0.92050000000000021</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E41" s="6">
         <v>1996</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G41" s="7">
         <f t="shared" si="2"/>
         <v>0.92420000000000024</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="42" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E42" s="6">
         <v>1997</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G42" s="7">
         <f t="shared" si="2"/>
         <v>0.92790000000000028</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E43" s="6">
         <v>1998</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G43" s="7">
         <f t="shared" si="2"/>
         <v>0.93160000000000032</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="44" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E44" s="6">
         <v>1999</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G44" s="7">
         <f t="shared" si="2"/>
         <v>0.93530000000000035</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E45" s="6">
         <v>2000</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G45" s="6">
         <f>C8</f>
         <v>0.93899999999999995</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="46" spans="5:8" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E46" s="6">
         <v>2001</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G46" s="7">
         <f>G45+(($G$55-$G$45)/($E$55-$E$45))</f>
         <v>0.94019999999999992</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="47" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E47" s="6">
         <v>2002</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G47" s="7">
         <f t="shared" ref="G47:G54" si="3">G46+(($G$55-$G$45)/($E$55-$E$45))</f>
         <v>0.9413999999999999</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="48" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E48" s="6">
         <v>2003</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G48" s="7">
         <f t="shared" si="3"/>
         <v>0.94259999999999988</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E49" s="6">
         <v>2004</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G49" s="7">
         <f t="shared" si="3"/>
         <v>0.94379999999999986</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E50" s="6">
         <v>2005</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G50" s="7">
         <f t="shared" si="3"/>
         <v>0.94499999999999984</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="51" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E51" s="6">
         <v>2006</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G51" s="7">
         <f t="shared" si="3"/>
         <v>0.94619999999999982</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="52" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E52" s="6">
         <v>2007</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G52" s="7">
         <f t="shared" si="3"/>
         <v>0.9473999999999998</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="53" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E53" s="6">
         <v>2008</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G53" s="7">
         <f t="shared" si="3"/>
         <v>0.94859999999999978</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="54" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E54" s="6">
         <v>2009</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G54" s="7">
         <f t="shared" si="3"/>
         <v>0.94979999999999976</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="55" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E55" s="6">
         <v>2010</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G55" s="6">
         <f>C9</f>
         <v>0.95099999999999996</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="56" spans="5:8" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E56" s="6">
         <v>2011</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G56" s="8">
         <f>G55+(($G$58-$G$55)/($E$58-$E$55))</f>
         <v>0.95333333333333325</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="57" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E57" s="6">
         <v>2012</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G57" s="8">
         <f>G56+(($G$58-$G$55)/($E$58-$E$55))</f>
         <v>0.95566666666666655</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="58" spans="5:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E58" s="6">
         <v>2013</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G58" s="6">
         <f>C10</f>
         <v>0.95799999999999996</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>